<commit_message>
Implementation of ticket buying.
</commit_message>
<xml_diff>
--- a/workbook.xlsx
+++ b/workbook.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Room1</t>
   </si>
   <si>
-    <t xml:space="preserve">Wizzard of Oz</t>
+    <t xml:space="preserve">Wizard of Oz</t>
   </si>
   <si>
     <t xml:space="preserve">Room2</t>
@@ -151,17 +151,14 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>